<commit_message>
Modified in Exponential ,Phantom Mismatch Data,Syteline Mapped data and writting failed
</commit_message>
<xml_diff>
--- a/Input_Automation/Phantom Items.xlsx
+++ b/Input_Automation/Phantom Items.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpadeveloper\Documents\UiPath\Fellowes_Validation\Input_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F03775-1FCC-479E-A0E1-64713CC78865}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FDF926-A81E-49AC-9738-CCD6B3C394C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="16110" windowHeight="6850" xr2:uid="{6ABD80F8-E04B-4DC7-BD19-74BFF736B6CF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="16110" windowHeight="6860" xr2:uid="{6ABD80F8-E04B-4DC7-BD19-74BFF736B6CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$708</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$716</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1868" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="696">
   <si>
     <t>Sl No</t>
   </si>
@@ -2092,6 +2092,30 @@
   </si>
   <si>
     <t>815058D1-J0M</t>
+  </si>
+  <si>
+    <t>(PHANTOM);EDGE;PVC;.9375 X.040 IN;E5</t>
+  </si>
+  <si>
+    <t>387881XY2</t>
+  </si>
+  <si>
+    <t>391856L</t>
+  </si>
+  <si>
+    <t>(PHANTOM);EDGE;PVC;.9375 X.040 IN;E3</t>
+  </si>
+  <si>
+    <t>387881XY0</t>
+  </si>
+  <si>
+    <t>387881E5</t>
+  </si>
+  <si>
+    <t>387881E3</t>
+  </si>
+  <si>
+    <t>38788100000</t>
   </si>
 </sst>
 </file>
@@ -2704,7 +2728,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2809,16 +2833,17 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3178,8 +3203,8 @@
   <dimension ref="A1:F725"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A690" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A708" sqref="A708:XFD708"/>
+      <pane ySplit="1" topLeftCell="A534" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D718" sqref="D718"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12176,18 +12201,18 @@
       <c r="A709" s="37">
         <v>300</v>
       </c>
-      <c r="B709" s="34" t="s">
+      <c r="B709" s="35" t="s">
         <v>677</v>
       </c>
-      <c r="C709" s="33" t="s">
+      <c r="C709" s="35" t="s">
         <v>678</v>
       </c>
-      <c r="D709" s="34" t="s">
+      <c r="D709" s="35" t="s">
         <v>679</v>
       </c>
     </row>
     <row r="710" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A710" s="39">
+      <c r="A710" s="37">
         <v>301</v>
       </c>
       <c r="B710" s="35" t="s">
@@ -12201,21 +12226,21 @@
       </c>
     </row>
     <row r="711" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A711" s="39">
+      <c r="A711" s="37">
         <v>302</v>
       </c>
-      <c r="B711" s="40" t="s">
+      <c r="B711" s="38" t="s">
         <v>682</v>
       </c>
-      <c r="C711" s="40" t="s">
+      <c r="C711" s="38" t="s">
         <v>683</v>
       </c>
-      <c r="D711" s="40" t="s">
+      <c r="D711" s="38" t="s">
         <v>684</v>
       </c>
     </row>
     <row r="712" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A712" s="41">
+      <c r="A712" s="37">
         <v>303</v>
       </c>
       <c r="B712" s="33" t="s">
@@ -12229,24 +12254,60 @@
       </c>
     </row>
     <row r="713" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A713" s="38"/>
-      <c r="B713" s="5"/>
-      <c r="C713" s="6"/>
+      <c r="A713" s="37">
+        <v>304</v>
+      </c>
+      <c r="B713" s="41" t="s">
+        <v>693</v>
+      </c>
+      <c r="C713" s="39" t="s">
+        <v>688</v>
+      </c>
+      <c r="D713" s="40" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="714" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A714" s="38"/>
-      <c r="B714" s="5"/>
-      <c r="C714" s="6"/>
+      <c r="A714" s="37">
+        <v>305</v>
+      </c>
+      <c r="B714" s="35" t="s">
+        <v>690</v>
+      </c>
+      <c r="C714" s="33" t="s">
+        <v>640</v>
+      </c>
+      <c r="D714" s="35" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="715" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A715" s="29"/>
-      <c r="B715" s="5"/>
-      <c r="C715" s="6"/>
+      <c r="A715" s="37">
+        <v>306</v>
+      </c>
+      <c r="B715" s="41" t="s">
+        <v>694</v>
+      </c>
+      <c r="C715" s="39" t="s">
+        <v>691</v>
+      </c>
+      <c r="D715" s="35" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="716" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A716" s="29"/>
-      <c r="B716" s="5"/>
-      <c r="C716" s="6"/>
+      <c r="A716" s="29">
+        <v>307</v>
+      </c>
+      <c r="B716" s="42" t="s">
+        <v>695</v>
+      </c>
+      <c r="C716" s="39" t="s">
+        <v>688</v>
+      </c>
+      <c r="D716" s="40" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="717" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A717" s="29"/>
@@ -12257,6 +12318,7 @@
       <c r="A718" s="29"/>
       <c r="B718" s="5"/>
       <c r="C718" s="6"/>
+      <c r="D718" s="42"/>
     </row>
     <row r="719" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A719" s="29"/>

</xml_diff>